<commit_message>
a big load of stuff omg
</commit_message>
<xml_diff>
--- a/Writing/Notes and files/Gantt Chart.xlsx
+++ b/Writing/Notes and files/Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\Final Year Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ruyak\Documents\University\Third Year\Final-Year-Project\Ruya Kumru-Holroyd\Ruya Kumru-Holroyd\Writing\Notes and files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D058CD27-4546-42D0-BC1C-6139271C486D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F315767E-6576-42E3-AED4-511A17E7EB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +182,13 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92CDDC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -315,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -406,6 +413,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,16 +1060,16 @@
       <c r="C5" s="31"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
-      <c r="F5" s="31"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
       <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
+      <c r="O5" s="50"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
       <c r="R5" s="29"/>
@@ -1163,12 +1172,12 @@
       <c r="E7" s="29"/>
       <c r="F7" s="31"/>
       <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
       <c r="P7" s="29"/>
@@ -1543,12 +1552,12 @@
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="29"/>
       <c r="O15" s="29"/>
       <c r="P15" s="29"/>
@@ -1622,7 +1631,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="31"/>
-      <c r="G17" s="29"/>
+      <c r="G17" s="31"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -1701,16 +1710,16 @@
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
       <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
       <c r="R19" s="29"/>
@@ -1784,9 +1793,9 @@
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
       <c r="N21" s="29"/>
@@ -1853,7 +1862,7 @@
       <c r="AH22" s="4"/>
       <c r="AI22" s="4"/>
     </row>
-    <row r="23" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30"/>
       <c r="B23" s="27" t="s">
         <v>3</v>
@@ -1865,9 +1874,9 @@
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
@@ -1958,11 +1967,11 @@
       <c r="H25" s="29"/>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
@@ -2064,9 +2073,9 @@
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="36"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="51"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
@@ -2167,10 +2176,10 @@
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
       <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
-      <c r="O29" s="29"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
       <c r="R29" s="29"/>
@@ -2272,9 +2281,9 @@
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
       <c r="P31" s="29"/>
       <c r="Q31" s="29"/>
       <c r="R31" s="29"/>
@@ -2376,9 +2385,9 @@
       <c r="J33" s="29"/>
       <c r="K33" s="29"/>
       <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="29"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="31"/>
+      <c r="O33" s="31"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
@@ -2794,7 +2803,7 @@
       <c r="L41" s="29"/>
       <c r="M41" s="29"/>
       <c r="N41" s="29"/>
-      <c r="O41" s="29"/>
+      <c r="O41" s="31"/>
       <c r="P41" s="29"/>
       <c r="Q41" s="29"/>
       <c r="R41" s="29"/>

</xml_diff>